<commit_message>
minor Excel format addition
</commit_message>
<xml_diff>
--- a/ITAD API.xlsx
+++ b/ITAD API.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="307">
   <si>
     <t>Webhooks</t>
   </si>
@@ -495,9 +495,6 @@
   </si>
   <si>
     <t>internal-twitchstream-v1</t>
-  </si>
-  <si>
-    <t>Page</t>
   </si>
   <si>
     <t>Deals-List</t>
@@ -1057,12 +1054,15 @@
 It is not necessary to have copy for each game in Collection, so you should not rely on this endpoint if you need to know about all games in user's Collection.
 CORRECTION: it gets all the copies the indicated games that the user has in collection.</t>
   </si>
+  <si>
+    <t>Endpoint2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,39 +1101,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1149,7 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1160,28 +1139,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1193,13 +1154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1211,14 +1166,183 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="32">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1446,20 +1570,15 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1552,24 +1671,6 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1584,7 +1685,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:Q63" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:Q63" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:Q63">
     <filterColumn colId="8">
       <filters>
@@ -1592,26 +1693,29 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A2:Q63">
+    <sortCondition ref="A1:A63"/>
+  </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="#" dataDxfId="16"/>
-    <tableColumn id="2" name="Duplicate" dataDxfId="15"/>
-    <tableColumn id="3" name="Group" dataDxfId="14"/>
-    <tableColumn id="4" name="Subgroup" dataDxfId="13"/>
-    <tableColumn id="6" name="Page" dataDxfId="12"/>
-    <tableColumn id="7" name="URL" dataDxfId="0" dataCellStyle="Hipervínculo">
+    <tableColumn id="1" name="#" dataDxfId="31"/>
+    <tableColumn id="2" name="Duplicate" dataDxfId="30"/>
+    <tableColumn id="3" name="Group" dataDxfId="29"/>
+    <tableColumn id="4" name="Subgroup" dataDxfId="28"/>
+    <tableColumn id="6" name="Endpoint" dataDxfId="27"/>
+    <tableColumn id="7" name="URL" dataDxfId="26" dataCellStyle="Hipervínculo">
       <calculatedColumnFormula>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Title" dataDxfId="11"/>
-    <tableColumn id="11" name="Description" dataDxfId="10"/>
-    <tableColumn id="9" name="Implem." dataDxfId="9"/>
-    <tableColumn id="16" name="Class Name" dataDxfId="8"/>
-    <tableColumn id="5" name="Type" dataDxfId="7"/>
-    <tableColumn id="17" name="Endpoint" dataDxfId="6"/>
-    <tableColumn id="10" name="Security" dataDxfId="5"/>
-    <tableColumn id="12" name="Query param_x000a_(key:API_KEY _x000a_+ ...)" dataDxfId="4"/>
-    <tableColumn id="15" name="Header param_x000a_(Authorization: TOKEN_x000a_'Content-Type':_x000a_+ …)" dataDxfId="3"/>
-    <tableColumn id="14" name="Body" dataDxfId="2"/>
-    <tableColumn id="13" name="Response" dataDxfId="1"/>
+    <tableColumn id="8" name="Title" dataDxfId="25"/>
+    <tableColumn id="11" name="Description" dataDxfId="24"/>
+    <tableColumn id="9" name="Implem." dataDxfId="23"/>
+    <tableColumn id="16" name="Class Name" dataDxfId="22"/>
+    <tableColumn id="5" name="Type" dataDxfId="21"/>
+    <tableColumn id="17" name="Endpoint2" dataDxfId="20"/>
+    <tableColumn id="10" name="Security" dataDxfId="19"/>
+    <tableColumn id="12" name="Query param_x000a_(key:API_KEY _x000a_+ ...)" dataDxfId="18"/>
+    <tableColumn id="15" name="Header param_x000a_(Authorization: TOKEN_x000a_'Content-Type':_x000a_+ …)" dataDxfId="17"/>
+    <tableColumn id="14" name="Body" dataDxfId="16"/>
+    <tableColumn id="13" name="Response" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1880,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,34 +1996,33 @@
     <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="42" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="60.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" style="3" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25.28515625" style="3" customWidth="1"/>
     <col min="20" max="20" width="22.42578125" style="3" customWidth="1"/>
     <col min="21" max="21" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="27.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
@@ -1928,7 +2031,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>254</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>37</v>
@@ -1936,43 +2039,43 @@
       <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1983,76 +2086,74 @@
       <c r="E2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="4" t="str">
-        <f t="shared" ref="F2:F33" si="0">HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</f>
+      <c r="F2" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>246</v>
+      <c r="H2" s="9" t="s">
+        <v>245</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="V2" s="3"/>
-    </row>
-    <row r="3" spans="1:22" s="5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D3,"/operation/",E3),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:22" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -2063,39 +2164,37 @@
       <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F4" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D4,"/operation/",E4),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>248</v>
+      <c r="H4" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="V4" s="3"/>
-    </row>
-    <row r="5" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -2106,39 +2205,37 @@
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F5" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D5,"/operation/",E5),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="V5" s="3"/>
-    </row>
-    <row r="6" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    </row>
+    <row r="6" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -2149,39 +2246,37 @@
       <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F6" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D6,"/operation/",E6),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="V6" s="3"/>
-    </row>
-    <row r="7" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>178</v>
+      <c r="B7" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -2189,54 +2284,53 @@
       <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" s="15" t="s">
+      <c r="F7" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D7,"/operation/",E7),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q7" s="13" t="s">
+      <c r="I7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="N7" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>178</v>
+      <c r="B8" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -2244,138 +2338,142 @@
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D8,"/operation/",E8),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="N8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="V8" s="3"/>
-    </row>
-    <row r="9" spans="1:22" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    </row>
+    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="F9" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D9,"/operation/",E9),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J9" s="8"/>
+      <c r="I9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J9" s="4"/>
       <c r="K9" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L9" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D10,"/operation/",E10),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="M9" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:22" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>172</v>
+      <c r="M10" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:22" ht="270" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" ht="270" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -2386,51 +2484,50 @@
       <c r="E11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F11" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D11,"/operation/",E11),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q11" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="V11" s="3"/>
-    </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -2441,39 +2538,37 @@
       <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F12" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D12,"/operation/",E12),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="V12" s="3"/>
-    </row>
-    <row r="13" spans="1:22" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -2484,39 +2579,37 @@
       <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F13" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D13,"/operation/",E13),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>249</v>
+      <c r="H13" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
@@ -2527,39 +2620,37 @@
       <c r="E14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F14" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D14,"/operation/",E14),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="V14" s="3"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -2570,39 +2661,37 @@
       <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F15" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D15,"/operation/",E15),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="7" t="s">
         <v>52</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="V15" s="3"/>
-    </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>2</v>
@@ -2613,39 +2702,37 @@
       <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F16" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D16,"/operation/",E16),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="7" t="s">
         <v>55</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="V16" s="3"/>
-    </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>2</v>
@@ -2656,82 +2743,78 @@
       <c r="E17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F17" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D17,"/operation/",E17),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="7" t="s">
         <v>96</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="V17" s="3"/>
-    </row>
-    <row r="18" spans="1:22" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F18" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D18,"/operation/",E18),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>250</v>
+      <c r="H18" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="V18" s="3"/>
-    </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -2742,1157 +2825,1138 @@
       <c r="E19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F19" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D19,"/operation/",E19),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="7" t="s">
         <v>99</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="V19" s="3"/>
-    </row>
-    <row r="20" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F20" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D20,"/operation/",E20),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="V20" s="3"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I20" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F21" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D21,"/operation/",E21),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P21" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V21" s="3"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I21" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F22" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D22,"/operation/",E22),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P22" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q22" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V22" s="3"/>
-    </row>
-    <row r="23" spans="1:22" s="8" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="I22" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D23,"/operation/",E23),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="I23" s="8" t="s">
+      <c r="H23" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>102</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>172</v>
+        <v>257</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:22" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+    <row r="24" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D24,"/operation/",E24),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="4" t="s">
         <v>102</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>172</v>
+        <v>257</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:22" s="8" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="F25" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D25,"/operation/",E25),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="I25" s="8" t="s">
+      <c r="H25" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>102</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>179</v>
+        <v>256</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:22" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Link</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="H26" s="16" t="s">
+      <c r="F26" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D26,"/operation/",E26),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J26" s="8"/>
+      <c r="I26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="4"/>
       <c r="K26" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>173</v>
+        <v>257</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:22" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F27" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F27" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D27,"/operation/",E27),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O27" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P27" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q27" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="V27" s="3"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I27" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F28" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D28,"/operation/",E28),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P28" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q28" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V28" s="3"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I28" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F29" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D29,"/operation/",E29),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P29" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V29" s="3"/>
-    </row>
-    <row r="30" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+      <c r="I29" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F30" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D30,"/operation/",E30),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J30" s="12" t="s">
+      <c r="H30" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O30" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="V30" s="3"/>
-    </row>
-    <row r="31" spans="1:22" ht="105" x14ac:dyDescent="0.25">
+      <c r="I30" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F31" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D31,"/operation/",E31),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O31" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P31" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q31" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V31" s="3"/>
-    </row>
-    <row r="32" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+      <c r="H31" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F32" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F32" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D32,"/operation/",E32),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P32" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q32" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V32" s="3"/>
-    </row>
-    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="H32" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F33" s="4" t="str">
-        <f t="shared" si="0"/>
+      <c r="F33" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D33,"/operation/",E33),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P33" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q33" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V33" s="3"/>
-    </row>
-    <row r="34" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="H33" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="4" t="str">
-        <f t="shared" ref="F34:F65" si="1">HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D34,"/operation/",E34),"Link")</f>
+      <c r="F34" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D34,"/operation/",E34),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q34" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="V34" s="3"/>
-    </row>
-    <row r="35" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="H34" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F35" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D35,"/operation/",E35),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H35" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P35" s="13" t="s">
+      <c r="H35" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="Q35" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="V35" s="3"/>
-    </row>
-    <row r="36" spans="1:22" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F36" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F36" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D36,"/operation/",E36),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O36" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P36" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q36" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="V36" s="3"/>
-    </row>
-    <row r="37" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="H36" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F37" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F37" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D37,"/operation/",E37),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q37" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V37" s="3"/>
-    </row>
-    <row r="38" spans="1:22" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="H37" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F38" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Link</v>
-      </c>
-      <c r="G38" s="8" t="s">
+      <c r="F38" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D38,"/operation/",E38),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="4" t="s">
         <v>102</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>172</v>
+        <v>257</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
     </row>
-    <row r="39" spans="1:22" s="5" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B39" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Link</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="F39" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D39,"/operation/",E39),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>172</v>
+      <c r="H39" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
     </row>
-    <row r="40" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+    <row r="40" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B40" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Link</v>
-      </c>
-      <c r="G40" s="5" t="s">
+      <c r="F40" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D40,"/operation/",E40),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>172</v>
+      <c r="I40" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
-    <row r="41" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+    <row r="41" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F41" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Link</v>
-      </c>
-      <c r="G41" s="5" t="s">
+      <c r="F41" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D41,"/operation/",E41),"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L41" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>172</v>
+      <c r="I41" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
     </row>
-    <row r="42" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>12</v>
@@ -3903,38 +3967,36 @@
       <c r="E42" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F42" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F42" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D42,"/operation/",E42),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="18" t="s">
-        <v>253</v>
+      <c r="H42" s="10" t="s">
+        <v>252</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L42" s="12" t="s">
-        <v>278</v>
+        <v>176</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="V42" s="3"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>13</v>
@@ -3945,216 +4007,212 @@
       <c r="E43" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F43" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F43" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D43,"/operation/",E43),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="H43" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="I43" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L43" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="M43" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N43" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O43" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P43" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q43" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="V43" s="3"/>
-    </row>
-    <row r="44" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="I43" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F44" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F44" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D44,"/operation/",E44),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I44" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O44" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P44" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q44" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="V44" s="3"/>
-    </row>
-    <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="I44" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F45" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F45" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D45,"/operation/",E45),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H45" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="M45" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N45" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O45" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P45" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q45" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V45" s="3"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H45" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F46" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D46,"/operation/",E46),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H46" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="K46" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="O46" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P46" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q46" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V46" s="3"/>
-    </row>
-    <row r="47" spans="1:22" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>13</v>
@@ -4165,38 +4223,36 @@
       <c r="E47" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F47" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F47" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D47,"/operation/",E47),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H47" s="19" t="s">
-        <v>241</v>
+      <c r="H47" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>293</v>
+        <v>176</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="V47" s="3"/>
-    </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>13</v>
@@ -4207,38 +4263,36 @@
       <c r="E48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F48" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F48" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D48,"/operation/",E48),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H48" s="19" t="s">
-        <v>166</v>
+      <c r="H48" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="L48" s="12" t="s">
-        <v>293</v>
+        <v>176</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="V48" s="3"/>
-    </row>
-    <row r="49" spans="1:22" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>13</v>
@@ -4249,51 +4303,50 @@
       <c r="E49" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F49" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F49" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D49,"/operation/",E49),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H49" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="K49" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="L49" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="M49" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O49" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="P49" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q49" s="6" t="s">
+      <c r="H49" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="P49" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="V49" s="3"/>
-    </row>
-    <row r="50" spans="1:22" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q49" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>13</v>
@@ -4304,51 +4357,50 @@
       <c r="E50" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F50" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F50" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D50,"/operation/",E50),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H50" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="K50" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="L50" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="M50" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="N50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O50" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="P50" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q50" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="V50" s="3"/>
-    </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q50" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>16</v>
@@ -4359,38 +4411,36 @@
       <c r="E51" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F51" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F51" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D51,"/operation/",E51),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H51" s="13" t="s">
+      <c r="H51" s="7" t="s">
         <v>142</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>301</v>
+        <v>176</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="V51" s="3"/>
-    </row>
-    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>178</v>
+      <c r="B52" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>16</v>
@@ -4401,38 +4451,36 @@
       <c r="E52" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F52" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D52,"/operation/",E52),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H52" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" s="12" t="s">
         <v>110</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>298</v>
+        <v>176</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="V52" s="3"/>
-    </row>
-    <row r="53" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>16</v>
@@ -4443,38 +4491,36 @@
       <c r="E53" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F53" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F53" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D53,"/operation/",E53),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="20" t="s">
+      <c r="H53" s="12" t="s">
         <v>144</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K53" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>296</v>
+        <v>176</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>295</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="V53" s="3"/>
-    </row>
-    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>16</v>
@@ -4485,38 +4531,36 @@
       <c r="E54" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F54" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F54" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D54,"/operation/",E54),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="12" t="s">
         <v>146</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K54" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="L54" s="12" t="s">
-        <v>297</v>
+        <v>176</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="V54" s="3"/>
-    </row>
-    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>17</v>
@@ -4525,40 +4569,38 @@
         <v>17</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F55" s="4" t="str">
-        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="F55" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D55,"/operation/",E55),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H55" s="20" t="s">
+      <c r="H55" s="12" t="s">
         <v>147</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K55" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>280</v>
+        <v>176</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="V55" s="3"/>
-    </row>
-    <row r="56" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>18</v>
@@ -4569,38 +4611,36 @@
       <c r="E56" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F56" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F56" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D56,"/operation/",E56),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H56" s="13" t="s">
-        <v>244</v>
+      <c r="H56" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L56" s="12" t="s">
-        <v>281</v>
+        <v>176</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>280</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="V56" s="3"/>
-    </row>
-    <row r="57" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>18</v>
@@ -4611,36 +4651,34 @@
       <c r="E57" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F57" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F57" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D57,"/operation/",E57),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H57" s="13"/>
+      <c r="H57" s="7"/>
       <c r="I57" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>282</v>
+        <v>176</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>281</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="V57" s="3"/>
-    </row>
-    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>18</v>
@@ -4651,36 +4689,34 @@
       <c r="E58" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F58" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F58" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D58,"/operation/",E58),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H58" s="13"/>
+      <c r="H58" s="7"/>
       <c r="I58" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L58" s="12" t="s">
-        <v>283</v>
+        <v>176</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="V58" s="3"/>
-    </row>
-    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>18</v>
@@ -4691,36 +4727,34 @@
       <c r="E59" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F59" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F59" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D59,"/operation/",E59),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H59" s="20"/>
+      <c r="H59" s="12"/>
       <c r="I59" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>284</v>
+        <v>176</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="V59" s="3"/>
-    </row>
-    <row r="60" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>18</v>
@@ -4731,38 +4765,36 @@
       <c r="E60" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F60" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F60" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D60,"/operation/",E60),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H60" s="13" t="s">
-        <v>245</v>
+      <c r="H60" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K60" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>285</v>
+        <v>176</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="V60" s="3"/>
-    </row>
-    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>18</v>
@@ -4773,36 +4805,34 @@
       <c r="E61" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F61" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F61" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D61,"/operation/",E61),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H61" s="13"/>
+      <c r="H61" s="7"/>
       <c r="I61" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K61" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L61" s="12" t="s">
-        <v>286</v>
+        <v>176</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="V61" s="3"/>
-    </row>
-    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>18</v>
@@ -4813,36 +4843,34 @@
       <c r="E62" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F62" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F62" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D62,"/operation/",E62),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H62" s="13"/>
+      <c r="H62" s="7"/>
       <c r="I62" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K62" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L62" s="12" t="s">
-        <v>287</v>
+        <v>176</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="V62" s="3"/>
-    </row>
-    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>18</v>
@@ -4853,31 +4881,47 @@
       <c r="E63" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F63" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="F63" s="13" t="str">
+        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D63,"/operation/",E63),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H63" s="13"/>
+      <c r="H63" s="7"/>
       <c r="I63" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K63" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="L63" s="12" t="s">
-        <v>288</v>
+        <v>176</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="V63" s="3"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B63">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I63">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"later"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
now all ITAD classed inherit from ITADBaseClass, added launch options file
</commit_message>
<xml_diff>
--- a/ITAD API.xlsx
+++ b/ITAD API.xlsx
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,8 +1999,8 @@
     <col min="5" max="5" width="29.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="60.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" style="3" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
updated, readme, docstring and excel
</commit_message>
<xml_diff>
--- a/ITAD API.xlsx
+++ b/ITAD API.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="310">
   <si>
     <t>Webhooks</t>
   </si>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t>OAuth</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Duplicate</t>
@@ -787,9 +784,6 @@
     <t>DelUserNotesFromGame</t>
   </si>
   <si>
-    <t>later</t>
-  </si>
-  <si>
     <t>SearchGames</t>
   </si>
   <si>
@@ -1056,6 +1050,25 @@
   </si>
   <si>
     <t>Endpoint2</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>[{id:SHOP_ID, 
+title:SHOP_TITLE,
+deals:DEALS_N,
+games:GAMES_N,
+update:UPD_DATE}]</t>
+  </si>
+  <si>
+    <t>GetShopsInfo</t>
+  </si>
+  <si>
+    <t>country:COUNTRY_CODE</t>
+  </si>
+  <si>
+    <t>no (duplicate)</t>
   </si>
 </sst>
 </file>
@@ -1178,173 +1191,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <b val="0"/>
@@ -1671,6 +1518,82 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1685,37 +1608,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:Q63" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:Q63">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:Q63" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:Q63"/>
   <sortState ref="A2:Q63">
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="#" dataDxfId="31"/>
-    <tableColumn id="2" name="Duplicate" dataDxfId="30"/>
-    <tableColumn id="3" name="Group" dataDxfId="29"/>
-    <tableColumn id="4" name="Subgroup" dataDxfId="28"/>
-    <tableColumn id="6" name="Endpoint" dataDxfId="27"/>
-    <tableColumn id="7" name="URL" dataDxfId="26" dataCellStyle="Hipervínculo">
+    <tableColumn id="1" name="#" dataDxfId="16"/>
+    <tableColumn id="2" name="Duplicate" dataDxfId="15"/>
+    <tableColumn id="3" name="Group" dataDxfId="14"/>
+    <tableColumn id="4" name="Subgroup" dataDxfId="13"/>
+    <tableColumn id="6" name="Endpoint" dataDxfId="12"/>
+    <tableColumn id="7" name="URL" dataDxfId="11" dataCellStyle="Hipervínculo">
       <calculatedColumnFormula>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Title" dataDxfId="25"/>
-    <tableColumn id="11" name="Description" dataDxfId="24"/>
-    <tableColumn id="9" name="Implem." dataDxfId="23"/>
-    <tableColumn id="16" name="Class Name" dataDxfId="22"/>
-    <tableColumn id="5" name="Type" dataDxfId="21"/>
-    <tableColumn id="17" name="Endpoint2" dataDxfId="20"/>
-    <tableColumn id="10" name="Security" dataDxfId="19"/>
-    <tableColumn id="12" name="Query param_x000a_(key:API_KEY _x000a_+ ...)" dataDxfId="18"/>
-    <tableColumn id="15" name="Header param_x000a_(Authorization: TOKEN_x000a_'Content-Type':_x000a_+ …)" dataDxfId="17"/>
-    <tableColumn id="14" name="Body" dataDxfId="16"/>
-    <tableColumn id="13" name="Response" dataDxfId="15"/>
+    <tableColumn id="8" name="Title" dataDxfId="10"/>
+    <tableColumn id="11" name="Description" dataDxfId="9"/>
+    <tableColumn id="9" name="Implem." dataDxfId="8"/>
+    <tableColumn id="16" name="Class Name" dataDxfId="7"/>
+    <tableColumn id="5" name="Type" dataDxfId="6"/>
+    <tableColumn id="17" name="Endpoint2" dataDxfId="5"/>
+    <tableColumn id="10" name="Security" dataDxfId="4"/>
+    <tableColumn id="12" name="Query param_x000a_(key:API_KEY _x000a_+ ...)" dataDxfId="3"/>
+    <tableColumn id="15" name="Header param_x000a_(Authorization: TOKEN_x000a_'Content-Type':_x000a_+ …)" dataDxfId="2"/>
+    <tableColumn id="14" name="Body" dataDxfId="1"/>
+    <tableColumn id="13" name="Response" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1986,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,8 +1916,8 @@
     <col min="5" max="5" width="29.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" style="3" bestFit="1" customWidth="1"/>
@@ -2019,10 +1936,10 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
@@ -2031,7 +1948,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>37</v>
@@ -2043,39 +1960,39 @@
         <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>169</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -2087,33 +2004,33 @@
         <v>94</v>
       </c>
       <c r="F2" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</f>
+        <f t="shared" ref="F2:F33" si="0">HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D2,"/operation/",E2),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
@@ -2125,35 +2042,35 @@
         <v>93</v>
       </c>
       <c r="F3" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D3,"/operation/",E3),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -2165,36 +2082,36 @@
         <v>29</v>
       </c>
       <c r="F4" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D4,"/operation/",E4),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>170</v>
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -2206,7 +2123,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D5,"/operation/",E5),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -2216,26 +2133,26 @@
         <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>170</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -2247,7 +2164,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D6,"/operation/",E6),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -2257,26 +2174,26 @@
         <v>41</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>170</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -2288,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D7,"/operation/",E7),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -2297,23 +2214,23 @@
       <c r="H7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>176</v>
+      <c r="I7" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>171</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>102</v>
@@ -2322,15 +2239,15 @@
         <v>102</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -2342,7 +2259,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D8,"/operation/",E8),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2352,27 +2269,27 @@
         <v>33</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="3" t="s">
         <v>102</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -2380,7 +2297,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
@@ -2392,7 +2309,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D9,"/operation/",E9),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -2402,20 +2319,20 @@
         <v>35</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>102</v>
@@ -2424,15 +2341,15 @@
         <v>102</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -2444,7 +2361,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D10,"/operation/",E10),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -2454,14 +2371,14 @@
         <v>33</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>171</v>
@@ -2473,7 +2390,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -2485,7 +2402,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D11,"/operation/",E11),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -2495,22 +2412,22 @@
         <v>40</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>171</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>102</v>
@@ -2519,15 +2436,15 @@
         <v>102</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -2539,7 +2456,7 @@
         <v>46</v>
       </c>
       <c r="F12" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D12,"/operation/",E12),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -2549,26 +2466,26 @@
         <v>42</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -2580,36 +2497,36 @@
         <v>44</v>
       </c>
       <c r="F13" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D13,"/operation/",E13),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
@@ -2621,7 +2538,7 @@
         <v>47</v>
       </c>
       <c r="F14" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D14,"/operation/",E14),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -2631,26 +2548,26 @@
         <v>49</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -2662,7 +2579,7 @@
         <v>50</v>
       </c>
       <c r="F15" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D15,"/operation/",E15),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -2672,26 +2589,26 @@
         <v>52</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>2</v>
@@ -2703,7 +2620,7 @@
         <v>53</v>
       </c>
       <c r="F16" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D16,"/operation/",E16),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -2713,26 +2630,26 @@
         <v>55</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>2</v>
@@ -2744,7 +2661,7 @@
         <v>95</v>
       </c>
       <c r="F17" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D17,"/operation/",E17),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -2754,26 +2671,26 @@
         <v>96</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>2</v>
@@ -2785,36 +2702,36 @@
         <v>97</v>
       </c>
       <c r="F18" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D18,"/operation/",E18),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>2</v>
@@ -2826,7 +2743,7 @@
         <v>98</v>
       </c>
       <c r="F19" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D19,"/operation/",E19),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -2836,14 +2753,14 @@
         <v>99</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>171</v>
@@ -2855,7 +2772,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -2867,7 +2784,7 @@
         <v>101</v>
       </c>
       <c r="F20" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D20,"/operation/",E20),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -2877,16 +2794,16 @@
         <v>100</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>172</v>
@@ -2901,7 +2818,7 @@
         <v>102</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2909,7 +2826,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
@@ -2921,7 +2838,7 @@
         <v>103</v>
       </c>
       <c r="F21" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D21,"/operation/",E21),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -2931,16 +2848,16 @@
         <v>104</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>172</v>
@@ -2952,7 +2869,7 @@
         <v>102</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>102</v>
@@ -2963,7 +2880,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
@@ -2975,7 +2892,7 @@
         <v>105</v>
       </c>
       <c r="F22" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D22,"/operation/",E22),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -2985,16 +2902,16 @@
         <v>106</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M22" s="6" t="s">
         <v>172</v>
@@ -3006,18 +2923,18 @@
         <v>102</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3029,23 +2946,23 @@
         <v>107</v>
       </c>
       <c r="F23" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D23,"/operation/",E23),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>171</v>
@@ -3055,12 +2972,12 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3072,7 +2989,7 @@
         <v>108</v>
       </c>
       <c r="F24" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D24,"/operation/",E24),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -3082,13 +2999,13 @@
         <v>109</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>171</v>
@@ -3098,12 +3015,12 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3115,38 +3032,38 @@
         <v>93</v>
       </c>
       <c r="F25" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D25,"/operation/",E25),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
@@ -3158,7 +3075,7 @@
         <v>111</v>
       </c>
       <c r="F26" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D26,"/operation/",E26),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3168,14 +3085,14 @@
         <v>110</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>172</v>
@@ -3187,7 +3104,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
@@ -3199,7 +3116,7 @@
         <v>112</v>
       </c>
       <c r="F27" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D27,"/operation/",E27),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -3209,16 +3126,16 @@
         <v>119</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>172</v>
@@ -3233,7 +3150,7 @@
         <v>102</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -3241,7 +3158,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
@@ -3253,7 +3170,7 @@
         <v>113</v>
       </c>
       <c r="F28" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D28,"/operation/",E28),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -3263,16 +3180,16 @@
         <v>120</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>172</v>
@@ -3284,7 +3201,7 @@
         <v>102</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>102</v>
@@ -3295,7 +3212,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>11</v>
@@ -3307,7 +3224,7 @@
         <v>121</v>
       </c>
       <c r="F29" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D29,"/operation/",E29),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -3317,16 +3234,16 @@
         <v>122</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>172</v>
@@ -3338,7 +3255,7 @@
         <v>102</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>102</v>
@@ -3349,7 +3266,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>11</v>
@@ -3361,26 +3278,26 @@
         <v>114</v>
       </c>
       <c r="F30" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D30,"/operation/",E30),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>172</v>
@@ -3392,10 +3309,10 @@
         <v>102</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q30" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="105" x14ac:dyDescent="0.25">
@@ -3403,7 +3320,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>11</v>
@@ -3415,26 +3332,26 @@
         <v>115</v>
       </c>
       <c r="F31" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D31,"/operation/",E31),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>172</v>
@@ -3446,7 +3363,7 @@
         <v>102</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>102</v>
@@ -3457,7 +3374,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>11</v>
@@ -3469,26 +3386,26 @@
         <v>116</v>
       </c>
       <c r="F32" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D32,"/operation/",E32),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>67</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>172</v>
@@ -3500,7 +3417,7 @@
         <v>102</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>102</v>
@@ -3511,7 +3428,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>11</v>
@@ -3523,26 +3440,26 @@
         <v>123</v>
       </c>
       <c r="F33" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D33,"/operation/",E33),"Link")</f>
+        <f t="shared" si="0"/>
         <v>Link</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>68</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>172</v>
@@ -3554,7 +3471,7 @@
         <v>102</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>102</v>
@@ -3565,7 +3482,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>11</v>
@@ -3577,26 +3494,26 @@
         <v>124</v>
       </c>
       <c r="F34" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D34,"/operation/",E34),"Link")</f>
+        <f t="shared" ref="F34:F65" si="1">HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D34,"/operation/",E34),"Link")</f>
         <v>Link</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>125</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>172</v>
@@ -3611,7 +3528,7 @@
         <v>102</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3619,7 +3536,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>11</v>
@@ -3631,26 +3548,26 @@
         <v>127</v>
       </c>
       <c r="F35" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D35,"/operation/",E35),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>172</v>
@@ -3662,10 +3579,10 @@
         <v>102</v>
       </c>
       <c r="P35" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="195" x14ac:dyDescent="0.25">
@@ -3673,7 +3590,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>11</v>
@@ -3685,26 +3602,26 @@
         <v>128</v>
       </c>
       <c r="F36" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D36,"/operation/",E36),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>172</v>
@@ -3716,10 +3633,10 @@
         <v>102</v>
       </c>
       <c r="P36" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -3727,7 +3644,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>11</v>
@@ -3739,26 +3656,26 @@
         <v>129</v>
       </c>
       <c r="F37" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D37,"/operation/",E37),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>70</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>172</v>
@@ -3770,18 +3687,18 @@
         <v>102</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q37" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>11</v>
@@ -3793,7 +3710,7 @@
         <v>130</v>
       </c>
       <c r="F38" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D38,"/operation/",E38),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -3803,13 +3720,13 @@
         <v>131</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>102</v>
+        <v>309</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>171</v>
@@ -3819,12 +3736,12 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>12</v>
@@ -3836,24 +3753,24 @@
         <v>107</v>
       </c>
       <c r="F39" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D39,"/operation/",E39),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>171</v>
@@ -3863,12 +3780,12 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>12</v>
@@ -3880,7 +3797,7 @@
         <v>108</v>
       </c>
       <c r="F40" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D40,"/operation/",E40),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -3890,14 +3807,14 @@
         <v>109</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>171</v>
@@ -3907,12 +3824,12 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>12</v>
@@ -3924,7 +3841,7 @@
         <v>130</v>
       </c>
       <c r="F41" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D41,"/operation/",E41),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -3934,14 +3851,14 @@
         <v>131</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>171</v>
@@ -3951,12 +3868,12 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
     </row>
-    <row r="42" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>12</v>
@@ -3968,35 +3885,35 @@
         <v>132</v>
       </c>
       <c r="F42" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D42,"/operation/",E42),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>72</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N42" s="3"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>13</v>
@@ -4008,7 +3925,7 @@
         <v>133</v>
       </c>
       <c r="F43" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D43,"/operation/",E43),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -4018,16 +3935,16 @@
         <v>134</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M43" s="6" t="s">
         <v>172</v>
@@ -4042,7 +3959,7 @@
         <v>102</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4050,7 +3967,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>13</v>
@@ -4062,7 +3979,7 @@
         <v>117</v>
       </c>
       <c r="F44" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D44,"/operation/",E44),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -4072,16 +3989,16 @@
         <v>135</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>172</v>
@@ -4096,7 +4013,7 @@
         <v>102</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4104,7 +4021,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>13</v>
@@ -4116,26 +4033,26 @@
         <v>118</v>
       </c>
       <c r="F45" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D45,"/operation/",E45),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>172</v>
@@ -4147,18 +4064,18 @@
         <v>102</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>13</v>
@@ -4170,26 +4087,26 @@
         <v>136</v>
       </c>
       <c r="F46" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D46,"/operation/",E46),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>76</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>172</v>
@@ -4201,18 +4118,18 @@
         <v>102</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>13</v>
@@ -4224,35 +4141,35 @@
         <v>137</v>
       </c>
       <c r="F47" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D47,"/operation/",E47),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N47" s="3"/>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>13</v>
@@ -4264,7 +4181,7 @@
         <v>138</v>
       </c>
       <c r="F48" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D48,"/operation/",E48),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -4274,25 +4191,25 @@
         <v>165</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M48" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N48" s="3"/>
     </row>
-    <row r="49" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>13</v>
@@ -4304,26 +4221,26 @@
         <v>139</v>
       </c>
       <c r="F49" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D49,"/operation/",E49),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>172</v>
@@ -4332,21 +4249,21 @@
         <v>102</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P49" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q49" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>13</v>
@@ -4358,26 +4275,26 @@
         <v>140</v>
       </c>
       <c r="F50" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D50,"/operation/",E50),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>172</v>
@@ -4386,21 +4303,21 @@
         <v>102</v>
       </c>
       <c r="O50" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P50" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q50" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>16</v>
@@ -4412,7 +4329,7 @@
         <v>141</v>
       </c>
       <c r="F51" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D51,"/operation/",E51),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G51" s="3" t="s">
@@ -4422,25 +4339,25 @@
         <v>142</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M51" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N51" s="3"/>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>16</v>
@@ -4452,7 +4369,7 @@
         <v>111</v>
       </c>
       <c r="F52" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D52,"/operation/",E52),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G52" s="3" t="s">
@@ -4462,25 +4379,25 @@
         <v>110</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M52" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N52" s="3"/>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>16</v>
@@ -4492,7 +4409,7 @@
         <v>143</v>
       </c>
       <c r="F53" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D53,"/operation/",E53),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G53" s="3" t="s">
@@ -4502,25 +4419,25 @@
         <v>144</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M53" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N53" s="3"/>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>16</v>
@@ -4532,7 +4449,7 @@
         <v>145</v>
       </c>
       <c r="F54" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D54,"/operation/",E54),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G54" s="3" t="s">
@@ -4542,25 +4459,25 @@
         <v>146</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M54" s="3" t="s">
         <v>172</v>
       </c>
       <c r="N54" s="3"/>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>17</v>
@@ -4572,7 +4489,7 @@
         <v>166</v>
       </c>
       <c r="F55" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D55,"/operation/",E55),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G55" s="3" t="s">
@@ -4582,25 +4499,39 @@
         <v>147</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>307</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="N55" s="3"/>
-    </row>
-    <row r="56" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q55" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>18</v>
@@ -4612,35 +4543,35 @@
         <v>148</v>
       </c>
       <c r="F56" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D56,"/operation/",E56),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>85</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="M56" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N56" s="3"/>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>18</v>
@@ -4652,7 +4583,7 @@
         <v>149</v>
       </c>
       <c r="F57" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D57,"/operation/",E57),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G57" s="3" t="s">
@@ -4660,25 +4591,25 @@
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N57" s="3"/>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>18</v>
@@ -4690,7 +4621,7 @@
         <v>150</v>
       </c>
       <c r="F58" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D58,"/operation/",E58),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G58" s="3" t="s">
@@ -4698,25 +4629,25 @@
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N58" s="3"/>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>18</v>
@@ -4728,7 +4659,7 @@
         <v>151</v>
       </c>
       <c r="F59" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D59,"/operation/",E59),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G59" s="3" t="s">
@@ -4736,25 +4667,25 @@
       </c>
       <c r="H59" s="12"/>
       <c r="I59" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N59" s="3"/>
     </row>
-    <row r="60" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>18</v>
@@ -4766,35 +4697,35 @@
         <v>152</v>
       </c>
       <c r="F60" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D60,"/operation/",E60),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>89</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N60" s="3"/>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>18</v>
@@ -4806,7 +4737,7 @@
         <v>153</v>
       </c>
       <c r="F61" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D61,"/operation/",E61),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G61" s="3" t="s">
@@ -4814,25 +4745,25 @@
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N61" s="3"/>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>18</v>
@@ -4844,7 +4775,7 @@
         <v>154</v>
       </c>
       <c r="F62" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D62,"/operation/",E62),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G62" s="3" t="s">
@@ -4852,25 +4783,25 @@
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M62" s="3" t="s">
         <v>171</v>
       </c>
       <c r="N62" s="3"/>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>18</v>
@@ -4882,7 +4813,7 @@
         <v>155</v>
       </c>
       <c r="F63" s="13" t="str">
-        <f>HYPERLINK(CONCATENATE("https://docs.isthereanydeal.com/#tag/",D63,"/operation/",E63),"Link")</f>
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
       <c r="G63" s="3" t="s">
@@ -4890,13 +4821,13 @@
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M63" s="3" t="s">
         <v>171</v>
@@ -4905,22 +4836,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B63">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="notEqual">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I63">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"later"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>